<commit_message>
Update New England Shelf to North East Shelf
</commit_message>
<xml_diff>
--- a/Data/AllFLPData.xlsx
+++ b/Data/AllFLPData.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://outlookuga-my.sharepoint.com/personal/ccz99536_uga_edu/Documents/Cruises/NES_CCS_Comparison/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://outlookuga-my.sharepoint.com/personal/ccz99536_uga_edu/Documents/Cruises/NES_CCS_Comparison/AcidotropicManuscript/AcidotropicDyes/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{5A03DA2A-0E95-D443-A3B2-FDC9CC4D82E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1775FD4-3AD6-7C45-9D29-44934E3D286F}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{5A03DA2A-0E95-D443-A3B2-FDC9CC4D82E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A74DCD8-BD18-114C-A4F6-EB89886CB2AA}"/>
   <bookViews>
     <workbookView xWindow="1900" yWindow="1820" windowWidth="27240" windowHeight="16440" xr2:uid="{ADC30944-6D44-A549-9F28-3103FD2E2AB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -92,9 +92,6 @@
     <t>X</t>
   </si>
   <si>
-    <t>New England Shelf</t>
-  </si>
-  <si>
     <t>SCM</t>
   </si>
   <si>
@@ -111,6 +108,9 @@
   </si>
   <si>
     <t>sdnoBR</t>
+  </si>
+  <si>
+    <t>North East Shelf</t>
   </si>
 </sst>
 </file>
@@ -485,8 +485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12413110-6882-AD43-8AF4-06A8DE2AFE67}">
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23:N36"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -526,16 +526,16 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" t="s">
         <v>21</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>22</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>23</v>
-      </c>
-      <c r="O1" t="s">
-        <v>24</v>
       </c>
       <c r="P1" t="s">
         <v>11</v>
@@ -1118,13 +1118,13 @@
         <v>0</v>
       </c>
       <c r="P12" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q12" t="s">
         <v>18</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="R12" t="s">
         <v>19</v>
-      </c>
-      <c r="R12" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
@@ -1162,13 +1162,13 @@
         <v>3.5764146584274701</v>
       </c>
       <c r="P13" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="Q13" t="s">
         <v>15</v>
       </c>
       <c r="R13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
@@ -1212,13 +1212,13 @@
         <v>33.7780976005659</v>
       </c>
       <c r="P14" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q14" t="s">
         <v>18</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="R14" t="s">
         <v>19</v>
-      </c>
-      <c r="R14" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
@@ -1262,13 +1262,13 @@
         <v>104.221137984802</v>
       </c>
       <c r="P15" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="Q15" t="s">
         <v>15</v>
       </c>
       <c r="R15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
@@ -1306,13 +1306,13 @@
         <v>32.412265620025202</v>
       </c>
       <c r="P16" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q16" t="s">
         <v>18</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="R16" t="s">
         <v>19</v>
-      </c>
-      <c r="R16" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
@@ -1326,13 +1326,13 @@
         <v>100156.17555710299</v>
       </c>
       <c r="P17" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="Q17" t="s">
         <v>15</v>
       </c>
       <c r="R17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
@@ -1370,13 +1370,13 @@
         <v>37.3499501690643</v>
       </c>
       <c r="P18" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q18" t="s">
         <v>18</v>
       </c>
-      <c r="Q18" t="s">
+      <c r="R18" t="s">
         <v>19</v>
-      </c>
-      <c r="R18" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
@@ -1414,13 +1414,13 @@
         <v>72.689710803721596</v>
       </c>
       <c r="P19" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="Q19" t="s">
         <v>15</v>
       </c>
       <c r="R19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.2">
@@ -1464,13 +1464,13 @@
         <v>69.875211721233399</v>
       </c>
       <c r="P20" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="Q20" t="s">
         <v>15</v>
       </c>
       <c r="R20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
@@ -1514,13 +1514,13 @@
         <v>206.157756550453</v>
       </c>
       <c r="P21" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q21" t="s">
         <v>18</v>
       </c>
-      <c r="Q21" t="s">
+      <c r="R21" t="s">
         <v>19</v>
-      </c>
-      <c r="R21" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
@@ -1564,13 +1564,13 @@
         <v>1229.08886646367</v>
       </c>
       <c r="P22" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="Q22" t="s">
         <v>15</v>
       </c>
       <c r="R22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
@@ -1578,13 +1578,13 @@
         <v>6</v>
       </c>
       <c r="P23" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="Q23" t="s">
         <v>15</v>
       </c>
       <c r="R23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
@@ -1592,13 +1592,13 @@
         <v>10</v>
       </c>
       <c r="P24" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="Q24" t="s">
         <v>15</v>
       </c>
       <c r="R24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
@@ -1622,10 +1622,10 @@
         <v>0.34987171580121001</v>
       </c>
       <c r="P25" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q25" t="s">
         <v>18</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>19</v>
       </c>
       <c r="R25" t="s">
         <v>16</v>
@@ -1642,7 +1642,7 @@
         <v>0</v>
       </c>
       <c r="P26" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="Q26" t="s">
         <v>15</v>
@@ -1665,17 +1665,17 @@
         <v>1.870169492</v>
       </c>
       <c r="H27">
-        <f t="shared" ref="H27:H37" si="0">LOG10(D27)</f>
+        <f t="shared" ref="H27:H32" si="0">LOG10(D27)</f>
         <v>0.27188096808978396</v>
       </c>
       <c r="J27">
         <v>0.17759363906612799</v>
       </c>
       <c r="P27" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q27" t="s">
         <v>18</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>19</v>
       </c>
       <c r="R27" t="s">
         <v>16</v>
@@ -1705,7 +1705,7 @@
         <v>0.57545479908400998</v>
       </c>
       <c r="P28" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="Q28" t="s">
         <v>15</v>
@@ -1735,10 +1735,10 @@
         <v>0.366810709845862</v>
       </c>
       <c r="P29" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q29" t="s">
         <v>18</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>19</v>
       </c>
       <c r="R29" t="s">
         <v>16</v>
@@ -1768,7 +1768,7 @@
         <v>1.2045381826283299</v>
       </c>
       <c r="P30" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="Q30" t="s">
         <v>15</v>
@@ -1801,10 +1801,10 @@
         <v>1.1024250379207501</v>
       </c>
       <c r="P31" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q31" t="s">
         <v>18</v>
-      </c>
-      <c r="Q31" t="s">
-        <v>19</v>
       </c>
       <c r="R31" t="s">
         <v>16</v>
@@ -1831,7 +1831,7 @@
         <v>1.1997636305463899</v>
       </c>
       <c r="P32" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="Q32" t="s">
         <v>15</v>
@@ -1851,7 +1851,7 @@
         <v>43124.7134615014</v>
       </c>
       <c r="P33" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="Q33" t="s">
         <v>15</v>
@@ -1877,10 +1877,10 @@
         <v>-3.3144401344741601</v>
       </c>
       <c r="P34" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q34" t="s">
         <v>18</v>
-      </c>
-      <c r="Q34" t="s">
-        <v>19</v>
       </c>
       <c r="R34" t="s">
         <v>16</v>
@@ -1897,7 +1897,7 @@
         <v>0</v>
       </c>
       <c r="P35" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="Q35" t="s">
         <v>15</v>
@@ -1911,7 +1911,7 @@
         <v>6</v>
       </c>
       <c r="P36" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="Q36" t="s">
         <v>15</v>
@@ -1925,7 +1925,7 @@
         <v>10</v>
       </c>
       <c r="P37" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="Q37" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
updates for new clarified dataframes
</commit_message>
<xml_diff>
--- a/Data/AllFLPData.xlsx
+++ b/Data/AllFLPData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://outlookuga-my.sharepoint.com/personal/ccz99536_uga_edu/Documents/Cruises/NES_CCS_Comparison/AcidotropicManuscript/AcidotropicDyes/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="8_{5A03DA2A-0E95-D443-A3B2-FDC9CC4D82E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D21AEAF8-CE3E-6D47-9D37-D59C0BBD4202}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="8_{5A03DA2A-0E95-D443-A3B2-FDC9CC4D82E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{156DC8C5-6379-AD49-9EDE-23E698427AAC}"/>
   <bookViews>
     <workbookView xWindow="30620" yWindow="-1460" windowWidth="23660" windowHeight="15900" xr2:uid="{ADC30944-6D44-A549-9F28-3103FD2E2AB5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="24">
   <si>
     <t>Station</t>
   </si>
@@ -105,9 +105,6 @@
   </si>
   <si>
     <t>North East Shelf</t>
-  </si>
-  <si>
-    <t>NA</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -488,8 +485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12413110-6882-AD43-8AF4-06A8DE2AFE67}">
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -711,7 +708,7 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -847,9 +844,6 @@
       </c>
       <c r="B8">
         <v>0.62305295950155803</v>
-      </c>
-      <c r="C8" t="s">
-        <v>23</v>
       </c>
       <c r="D8">
         <v>24.933079365079401</v>

</xml_diff>